<commit_message>
fixed 2 background hits from 5 day to 1 day hitcount
</commit_message>
<xml_diff>
--- a/Measurement.xlsx
+++ b/Measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\balazzs\HPGECalorimeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CB3221-18B2-41C8-BD9C-67C88CE579EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C6AA25-6B29-4D72-BD41-589525CAB3BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46746E60-17A0-4365-A090-14C1EF1167C0}"/>
   </bookViews>
@@ -427,7 +427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35189D99-37F1-49BD-9DAD-CAC80A16A5C4}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -526,7 +528,7 @@
         <v>6130</v>
       </c>
       <c r="F5">
-        <v>280</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -574,7 +576,7 @@
         <v>350</v>
       </c>
       <c r="F8">
-        <v>275</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>